<commit_message>
Taart chart gemaakt , Bar chart weggehaald. Alles van de BarChart is gecomment, maar nog niet weggehaald. Ilias gaat er nog naar kijken.  3169
</commit_message>
<xml_diff>
--- a/Bagage.xlsx
+++ b/Bagage.xlsx
@@ -115,6 +115,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -147,7 +150,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -465,7 +468,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,7 +590,7 @@
         <v>0.54236111111111118</v>
       </c>
       <c r="O2" s="2">
-        <v>43132</v>
+        <v>43114</v>
       </c>
       <c r="P2" t="s">
         <v>26</v>
@@ -601,5 +604,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel import is klaar!
</commit_message>
<xml_diff>
--- a/Bagage.xlsx
+++ b/Bagage.xlsx
@@ -116,7 +116,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="166" formatCode="d/mm/yy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -150,7 +150,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -468,7 +468,7 @@
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>